<commit_message>
Updating Unit 1 materials
</commit_message>
<xml_diff>
--- a/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/04-Par_Dartville/Unsolved/Dartville.xlsx
+++ b/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/04-Par_Dartville/Unsolved/Dartville.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\Documents\GitHub\GWU-ARL-DATA-PT-09-2019-U-C\01-Class-Activities\Mon-Wed-Class\01-Excel\3\Activities\04-Par_Dartville\Solved\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\Documents\GitHub\GWU-ARL-DATA-PT-09-2019-U-C\01-Class-Activities\Mon-Wed-Class\01-Excel\3\Activities\04-Par_Dartville\Unsolved\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="294">
   <si>
     <t>Aaron</t>
   </si>
@@ -738,12 +738,6 @@
     <t>Primary Phone</t>
   </si>
   <si>
-    <t>Highlight the fierce people in RED</t>
-  </si>
-  <si>
-    <t>Name formatted as "[Last], [First] [Middle]", for example "Williams, Dartanion De Angelo"</t>
-  </si>
-  <si>
     <t>(991) 473-7167</t>
   </si>
   <si>
@@ -909,9 +903,6 @@
     <t>(991) 724-4433</t>
   </si>
   <si>
-    <t>Special exercise: create a full report</t>
-  </si>
-  <si>
     <t>Full Name</t>
   </si>
   <si>
@@ -925,12 +916,6 @@
   </si>
   <si>
     <t>Age</t>
-  </si>
-  <si>
-    <t>Now I want to test your resourcefulness… figure out how to calculate age</t>
-  </si>
-  <si>
-    <t>Turn this into a formatted table</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1015,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1157,8 +1145,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1177,8 +1165,8 @@
   <autoFilter ref="A1:C56"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Student ID"/>
-    <tableColumn id="6" name="Birth Date" dataDxfId="6"/>
-    <tableColumn id="7" name="Gender" dataDxfId="5"/>
+    <tableColumn id="6" name="Birth Date" dataDxfId="7"/>
+    <tableColumn id="7" name="Gender" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1193,35 +1181,36 @@
     <tableColumn id="3" name="City"/>
     <tableColumn id="4" name="State"/>
     <tableColumn id="5" name="Zip"/>
-    <tableColumn id="6" name="Primary Phone" dataDxfId="4"/>
+    <tableColumn id="6" name="Primary Phone" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B56" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B56" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:B56"/>
   <sortState ref="A2:B56">
     <sortCondition ref="B1:B56"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Student ID" dataDxfId="1"/>
-    <tableColumn id="2" name="Diagnosis" dataDxfId="0"/>
+    <tableColumn id="1" name="Student ID" dataDxfId="2"/>
+    <tableColumn id="2" name="Diagnosis" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E60" totalsRowShown="0">
-  <autoFilter ref="A1:E60"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F60" totalsRowShown="0">
+  <autoFilter ref="A1:F60"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Student ID"/>
     <tableColumn id="8" name="Gender"/>
     <tableColumn id="2" name="Last Name"/>
     <tableColumn id="3" name="First Name"/>
     <tableColumn id="7" name="Middle Name"/>
+    <tableColumn id="4" name="Full Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1529,7 +1518,9 @@
   </sheetPr>
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2156,8 +2147,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2221,7 +2213,7 @@
         <v>20078</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2241,7 +2233,7 @@
         <v>20076</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2261,7 +2253,7 @@
         <v>20070</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2281,7 +2273,7 @@
         <v>20076</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2301,7 +2293,7 @@
         <v>20076</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2321,7 +2313,7 @@
         <v>20073</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2341,7 +2333,7 @@
         <v>20072</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2361,7 +2353,7 @@
         <v>20074</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2381,7 +2373,7 @@
         <v>20075</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2401,7 +2393,7 @@
         <v>20075</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2421,7 +2413,7 @@
         <v>20073</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2441,7 +2433,7 @@
         <v>20071</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2461,7 +2453,7 @@
         <v>20070</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,7 +2473,7 @@
         <v>20070</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2501,7 +2493,7 @@
         <v>20077</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2521,7 +2513,7 @@
         <v>20078</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2541,7 +2533,7 @@
         <v>20076</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2561,7 +2553,7 @@
         <v>20079</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2581,7 +2573,7 @@
         <v>20076</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2601,7 +2593,7 @@
         <v>20074</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2621,7 +2613,7 @@
         <v>20074</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2641,7 +2633,7 @@
         <v>20074</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2661,7 +2653,7 @@
         <v>20079</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2681,7 +2673,7 @@
         <v>20079</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2701,7 +2693,7 @@
         <v>20072</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2721,7 +2713,7 @@
         <v>20074</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2741,7 +2733,7 @@
         <v>20077</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2761,7 +2753,7 @@
         <v>20070</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2781,7 +2773,7 @@
         <v>20078</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2801,7 +2793,7 @@
         <v>20077</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2821,7 +2813,7 @@
         <v>20076</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,7 +2833,7 @@
         <v>20070</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2861,7 +2853,7 @@
         <v>20078</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2881,7 +2873,7 @@
         <v>20072</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2901,7 +2893,7 @@
         <v>20074</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2921,7 +2913,7 @@
         <v>20075</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2941,7 +2933,7 @@
         <v>20079</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2961,7 +2953,7 @@
         <v>20078</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2981,7 +2973,7 @@
         <v>20073</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3001,7 +2993,7 @@
         <v>20073</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3021,7 +3013,7 @@
         <v>20071</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3041,7 +3033,7 @@
         <v>20075</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -3061,7 +3053,7 @@
         <v>20071</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3081,7 +3073,7 @@
         <v>20079</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -3101,7 +3093,7 @@
         <v>20071</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -3121,7 +3113,7 @@
         <v>20074</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3141,7 +3133,7 @@
         <v>20074</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3161,7 +3153,7 @@
         <v>20070</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3181,7 +3173,7 @@
         <v>20078</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3201,7 +3193,7 @@
         <v>20077</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -3221,7 +3213,7 @@
         <v>20075</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3241,7 +3233,7 @@
         <v>20071</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3261,7 +3253,7 @@
         <v>20073</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -3281,7 +3273,7 @@
         <v>20075</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -3301,7 +3293,7 @@
         <v>20073</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -3790,7 +3782,7 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3803,7 +3795,7 @@
     <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -3819,8 +3811,11 @@
       <c r="E1" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>25012794</v>
       </c>
@@ -3837,7 +3832,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>25018253</v>
       </c>
@@ -3854,7 +3849,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>25011190</v>
       </c>
@@ -3871,7 +3866,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25012819</v>
       </c>
@@ -3888,7 +3883,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25016539</v>
       </c>
@@ -3905,7 +3900,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25014751</v>
       </c>
@@ -3922,7 +3917,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25018014</v>
       </c>
@@ -3939,7 +3934,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>25011994</v>
       </c>
@@ -3956,7 +3951,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>25013750</v>
       </c>
@@ -3973,7 +3968,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25011962</v>
       </c>
@@ -3990,7 +3985,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25007190</v>
       </c>
@@ -4007,7 +4002,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25016020</v>
       </c>
@@ -4024,7 +4019,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>25016460</v>
       </c>
@@ -4041,7 +4036,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>25015674</v>
       </c>
@@ -4058,7 +4053,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>25008738</v>
       </c>
@@ -4770,8 +4765,8 @@
   </sheetPr>
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L1:L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4792,203 +4787,193 @@
         <v>160</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>165</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>291</v>
-      </c>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="L2" s="7" t="s">
-        <v>235</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="L3" s="7" t="s">
-        <v>234</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="L4" s="7" t="s">
-        <v>297</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="L5" s="7" t="s">
-        <v>298</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="1"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="1"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="1"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="1"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="1"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="1"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="1"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="A34" s="1"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="A35" s="1"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="1"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="1"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="1"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="1"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
+      <c r="A50" s="1"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+      <c r="A51" s="1"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
+      <c r="A52" s="1"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
+      <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+      <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>

</xml_diff>